<commit_message>
change number to string
</commit_message>
<xml_diff>
--- a/DataSet/SignIn.xlsx
+++ b/DataSet/SignIn.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="11220" yWindow="460" windowWidth="27160" windowHeight="20000" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="20000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sign In" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="47">
   <si>
     <t>Internal ID</t>
   </si>
@@ -159,6 +159,12 @@
   </si>
   <si>
     <t>Please enter a valid email address.</t>
+  </si>
+  <si>
+    <t>12345678</t>
+  </si>
+  <si>
+    <t>1234567890</t>
   </si>
 </sst>
 </file>
@@ -240,9 +246,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -524,7 +530,7 @@
   <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -579,8 +585,8 @@
       <c r="C3" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D3">
-        <v>12345678</v>
+      <c r="D3" s="6" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="17" x14ac:dyDescent="0.2">
@@ -629,8 +635,8 @@
       <c r="C7" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D7">
-        <v>12345678</v>
+      <c r="D7" s="6" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="17" x14ac:dyDescent="0.2">
@@ -643,8 +649,8 @@
       <c r="C8" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="D8">
-        <v>12345678</v>
+      <c r="D8" s="6" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="17" x14ac:dyDescent="0.2">
@@ -657,15 +663,15 @@
       <c r="C9" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="D9">
-        <v>12345678</v>
+      <c r="D9" s="6" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="8" t="s">
         <v>10</v>
       </c>
       <c r="C10" s="5"/>
@@ -674,7 +680,7 @@
       <c r="A11" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B11" s="9" t="s">
+      <c r="B11" s="8" t="s">
         <v>11</v>
       </c>
     </row>
@@ -688,8 +694,8 @@
       <c r="C12" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D12">
-        <v>12345678</v>
+      <c r="D12" s="6" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="17" x14ac:dyDescent="0.2">
@@ -702,10 +708,10 @@
       <c r="C13" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D13">
-        <v>1234567890</v>
-      </c>
-      <c r="F13" s="8" t="s">
+      <c r="D13" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="F13" s="7" t="s">
         <v>43</v>
       </c>
     </row>
@@ -719,10 +725,10 @@
       <c r="C14" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="D14">
-        <v>12345678</v>
-      </c>
-      <c r="F14" s="8" t="s">
+      <c r="D14" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="F14" s="7" t="s">
         <v>43</v>
       </c>
     </row>
@@ -736,10 +742,10 @@
       <c r="C15" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="D15">
-        <v>1234567890</v>
-      </c>
-      <c r="F15" s="8" t="s">
+      <c r="D15" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="F15" s="7" t="s">
         <v>43</v>
       </c>
     </row>
@@ -753,10 +759,10 @@
       <c r="C16" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="D16" s="7">
-        <v>12345678</v>
-      </c>
-      <c r="F16" s="8" t="s">
+      <c r="D16" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="F16" s="7" t="s">
         <v>44</v>
       </c>
     </row>

</xml_diff>